<commit_message>
nothing changed, just experiments
</commit_message>
<xml_diff>
--- a/pics/simulations/FLMPC/tests_flmpc.xlsx
+++ b/pics/simulations/FLMPC/tests_flmpc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pindiche\Desktop\QcarProject\pics\simulations\FLMPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF482512-138C-4737-BB37-0956A8878696}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0CB80E-4DEA-4497-B072-DBBAF6EC41A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{468E8241-07BD-4C8D-B197-99E2DBA51C17}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>Test cases</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Tracking Err</t>
   </si>
   <si>
-    <t>Sampling Time</t>
-  </si>
-  <si>
-    <t>Ts = 0.1</t>
-  </si>
-  <si>
     <t>Simulation Time</t>
   </si>
   <si>
@@ -82,6 +76,15 @@
   </si>
   <si>
     <t>Q = diag(5,5)</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Nonlinear</t>
+  </si>
+  <si>
+    <t>Linear</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -240,12 +243,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -580,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C489DF-418A-40E7-8921-174EBB1C600C}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,36 +595,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="7"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>3</v>
@@ -635,49 +632,67 @@
       <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>17</v>
+      <c r="A5" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="10">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8">
         <v>1.6899999999999998E-2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>0.20499999999999999</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.1709</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="16"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="14"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -686,7 +701,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -699,13 +714,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
@@ -720,22 +735,22 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>17</v>
+      <c r="A11" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>0.22059999999999999</v>
       </c>
       <c r="G11" s="2"/>
@@ -745,12 +760,24 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1.5900000000000001E-2</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -765,11 +792,11 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,13 +804,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
@@ -793,39 +820,51 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>17</v>
+      <c r="A17" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.56920000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F17" s="10">
-        <v>0.56920000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="D18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.44269999999999998</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,13 +872,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>3</v>
@@ -849,23 +888,43 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>17</v>
+      <c r="A23" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.18779999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="10">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="F23" s="10">
-        <v>0.18779999999999999</v>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.13220000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>